<commit_message>
cambio en el caso de uso tarea
</commit_message>
<xml_diff>
--- a/análisis/Casos de Uso Narrativos/CDUN - (Tarea) Eliminar tarea.xlsx
+++ b/análisis/Casos de Uso Narrativos/CDUN - (Tarea) Eliminar tarea.xlsx
@@ -585,9 +585,6 @@
     <t>Eliminar tarea</t>
   </si>
   <si>
-    <t>4.4</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -634,6 +631,9 @@
   </si>
   <si>
     <t>Una tarea puede ser eliminada, independiente de su estado (realizada, no realizada, pendiente).</t>
+  </si>
+  <si>
+    <t>4.5</t>
   </si>
 </sst>
 </file>
@@ -1055,18 +1055,28 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1076,18 +1086,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1371,7 +1371,7 @@
   <dimension ref="B1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:I30"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1388,341 +1388,354 @@
   <sheetData>
     <row r="1" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="39"/>
       <c r="I2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="34"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18" t="s">
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="39">
+      <c r="G8" s="11">
         <v>42114</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="30"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33"/>
+      <c r="B11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="30"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="33"/>
+      <c r="B14" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="22"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="29"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="36"/>
+      <c r="C17" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="6">
         <v>2</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="37"/>
+      <c r="G17" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="25"/>
     </row>
     <row r="18" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>3</v>
       </c>
-      <c r="C18" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="38"/>
-      <c r="E18" s="33"/>
+      <c r="C18" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="26"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="7">
         <v>4</v>
       </c>
-      <c r="G18" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
+      <c r="G18" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="14"/>
     </row>
     <row r="19" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8"/>
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="30"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="17"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="19"/>
+        <v>35</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="33"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="14"/>
     </row>
     <row r="23" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="30"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="17"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="20"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="I26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I26" s="20"/>
     </row>
     <row r="27" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="32" t="s">
+      <c r="F27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="33"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="14"/>
     </row>
     <row r="28" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="30"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="17"/>
     </row>
     <row r="30" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="33"/>
+      <c r="B30" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="H26:I26"/>
@@ -1737,24 +1750,11 @@
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B30:I30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>